<commit_message>
Adding data and classifier
</commit_message>
<xml_diff>
--- a/rna_junctions.xlsx
+++ b/rna_junctions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benfeard/Documents/GitHub/learning_RNA_3way_junctions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABF5053-489C-564F-9B3D-9294AE216305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F95FD2-0B2A-5C46-97E6-AE9E7A712A50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6380" windowWidth="19460" windowHeight="16040" xr2:uid="{353F324F-3244-4946-A8BE-989828C3B852}"/>
+    <workbookView xWindow="0" yWindow="3420" windowWidth="25200" windowHeight="16040" xr2:uid="{353F324F-3244-4946-A8BE-989828C3B852}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>rna_label</t>
   </si>
@@ -58,6 +58,33 @@
   </si>
   <si>
     <t>junction_c</t>
+  </si>
+  <si>
+    <t>source_name</t>
+  </si>
+  <si>
+    <t>GGCGCU</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>GCCUGCAGGC</t>
+  </si>
+  <si>
+    <t>UA</t>
+  </si>
+  <si>
+    <t>GACGUG</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Family_A</t>
+  </si>
+  <si>
+    <t>16S H20-H21-H22</t>
   </si>
 </sst>
 </file>
@@ -409,38 +436,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B985E4F-3CD4-B04B-BF2A-A7F154281CD1}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>